<commit_message>
SSDM-6064 - more tweaks + first results
</commit_message>
<xml_diff>
--- a/openbis_benchmark/conf/results.xlsx
+++ b/openbis_benchmark/conf/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanf/Documents/programming/openbis_eclipse_workspace_git/openbis_benchmark/conf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{25C4C791-A782-5042-B807-1B51A9825ECF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F25E2D50-2A7E-A646-AC71-9FF0D3A74A0C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32880" yWindow="2540" windowWidth="45180" windowHeight="19280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29360" yWindow="460" windowWidth="50100" windowHeight="26140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>16
 shared_buffers 4GB
@@ -44,9 +44,6 @@
     <t>NOTES</t>
   </si>
   <si>
-    <t>SEARCH 50 : 7 THREADS BROKE</t>
-  </si>
-  <si>
     <t>LOAD</t>
   </si>
   <si>
@@ -57,12 +54,6 @@
   </si>
   <si>
     <t>RESULTS</t>
-  </si>
-  <si>
-    <t>TOTAL TIME</t>
-  </si>
-  <si>
-    <t>AVG SINGLE OP TIME</t>
   </si>
   <si>
     <t>THEADS</t>
@@ -84,6 +75,27 @@
   </si>
   <si>
     <t>OS MEM (GB)</t>
+  </si>
+  <si>
+    <t>TOTAL CPU TIME</t>
+  </si>
+  <si>
+    <t>TOTAL REAL TIME</t>
+  </si>
+  <si>
+    <t>TOTAL REAL AVG TIME</t>
+  </si>
+  <si>
+    <t>NUM OPERATIONS</t>
+  </si>
+  <si>
+    <t>AVG OPERATION TIME</t>
+  </si>
+  <si>
+    <t>MAX OPERATION TIME</t>
+  </si>
+  <si>
+    <t>MIN OPERATION TIME</t>
   </si>
 </sst>
 </file>
@@ -246,11 +258,19 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>LOAD -</a:t>
+              <a:t>LOAD</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> 16 CORES - 64GB</a:t>
+              <a:t> - </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>16 CPU</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> - 64 GB</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -296,11 +316,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$2</c:f>
+              <c:f>Sheet1!$G$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>THEADS</c:v>
+                  <c:v>TOTAL REAL TIME</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -317,7 +337,7 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:val>
+          <c:cat>
             <c:numRef>
               <c:f>Sheet1!$H$2:$L$2</c:f>
               <c:numCache>
@@ -340,11 +360,35 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$3:$L$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>107488</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>116416</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>123916</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>239546</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>542936</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-393D-2844-85A1-6F420394E35C}"/>
+              <c16:uniqueId val="{00000000-F94C-CF47-8596-1FED1861CCB8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -357,7 +401,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AVG SINGLE OP TIME</c:v>
+                  <c:v>TOTAL REAL AVG TIME</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -374,6 +418,30 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$L$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$H$4:$L$4</c:f>
@@ -381,19 +449,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>6.0385</c:v>
+                  <c:v>26872</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.21987</c:v>
+                  <c:v>5820</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6532</c:v>
+                  <c:v>3097</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.62802250000000004</c:v>
+                  <c:v>2994</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.58271800000000007</c:v>
+                  <c:v>2714</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -401,7 +469,250 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-393D-2844-85A1-6F420394E35C}"/>
+              <c16:uniqueId val="{00000001-F94C-CF47-8596-1FED1861CCB8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AVG OPERATION TIME</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$L$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$7:$L$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>26180</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28074</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29771</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>53364</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90123</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F94C-CF47-8596-1FED1861CCB8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MAX OPERATION TIME</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$L$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$8:$L$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>28253</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29664</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32226</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>86916</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>138099</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-F94C-CF47-8596-1FED1861CCB8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MIN OPERATION TIME</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$L$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$9:$L$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>24129</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25778</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27654</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33259</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29712</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-F94C-CF47-8596-1FED1861CCB8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -414,11 +725,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="75393727"/>
-        <c:axId val="75374399"/>
+        <c:axId val="313482463"/>
+        <c:axId val="260409007"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="75393727"/>
+        <c:axId val="313482463"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -461,7 +772,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75374399"/>
+        <c:crossAx val="260409007"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -469,7 +780,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75374399"/>
+        <c:axId val="260409007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -520,7 +831,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75393727"/>
+        <c:crossAx val="313482463"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -642,13 +953,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>SEARCH</a:t>
+              <a:t>QUERY - 16 CPU - 64 GB</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> - 16 CORES - 64 GB</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -692,11 +998,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$2</c:f>
+              <c:f>Sheet1!$G$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>THEADS</c:v>
+                  <c:v>AVG OPERATION TIME</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -713,9 +1019,9 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:val>
+          <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$M$2:$Q$2</c:f>
+              <c:f>Sheet1!$R$2:$V$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -733,6 +1039,30 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$7:$V$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>329</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>241</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>368</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -740,7 +1070,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4354-FB4F-B0AA-7774326E112D}"/>
+              <c16:uniqueId val="{00000000-826D-CC48-8555-1F3A867D26AE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -749,11 +1079,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$4</c:f>
+              <c:f>Sheet1!$G$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AVG SINGLE OP TIME</c:v>
+                  <c:v>MAX OPERATION TIME</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -770,26 +1100,50 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:val>
+          <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$M$4:$Q$4</c:f>
+              <c:f>Sheet1!$R$2:$V$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>6282.2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4017.44</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3884.1800000000003</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2556.98</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2774.4839999999999</c:v>
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$8:$V$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1796</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1481</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3843</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -797,7 +1151,88 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-4354-FB4F-B0AA-7774326E112D}"/>
+              <c16:uniqueId val="{00000001-826D-CC48-8555-1F3A867D26AE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MIN OPERATION TIME</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$R$2:$V$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$9:$V$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-826D-CC48-8555-1F3A867D26AE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -810,16 +1245,17 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="109822975"/>
-        <c:axId val="136413119"/>
+        <c:axId val="266195471"/>
+        <c:axId val="321183391"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="109822975"/>
+        <c:axId val="266195471"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -856,7 +1292,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="136413119"/>
+        <c:crossAx val="321183391"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -864,7 +1300,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="136413119"/>
+        <c:axId val="321183391"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -915,7 +1351,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="109822975"/>
+        <c:crossAx val="266195471"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1037,8 +1473,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>QUERY - 16 CORES - 64 GB</a:t>
+              <a:t>SEARCH</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> - 16 CPU - 64 GB</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1082,11 +1523,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$2</c:f>
+              <c:f>Sheet1!$G$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>THEADS</c:v>
+                  <c:v>AVG OPERATION TIME</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1103,9 +1544,9 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:val>
+          <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$V$2</c:f>
+              <c:f>Sheet1!$M$2:$Q$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1123,6 +1564,30 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$7:$Q$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2360</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11745</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>56646</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>63651</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46679</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1130,7 +1595,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-77A1-D947-B041-BEC1B0D1E271}"/>
+              <c16:uniqueId val="{00000000-CF98-4D44-BBE6-989CABA68FE5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1139,11 +1604,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$4</c:f>
+              <c:f>Sheet1!$G$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AVG SINGLE OP TIME</c:v>
+                  <c:v>MAX OPERATION TIME</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1160,26 +1625,50 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:val>
+          <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$R$4:$V$4</c:f>
+              <c:f>Sheet1!$M$2:$Q$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2343.8000000000002</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>169.06</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>122.35</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>96.24</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>272.19400000000002</c:v>
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$8:$Q$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3809</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>351279</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>473618</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>587264</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>565492</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1187,7 +1676,88 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-77A1-D947-B041-BEC1B0D1E271}"/>
+              <c16:uniqueId val="{00000001-CF98-4D44-BBE6-989CABA68FE5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MIN OPERATION TIME</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$M$2:$Q$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$9:$Q$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1399</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1464</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3770</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5432</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-CF98-4D44-BBE6-989CABA68FE5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1200,16 +1770,17 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="137051295"/>
-        <c:axId val="136882127"/>
+        <c:axId val="321536767"/>
+        <c:axId val="317453567"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="137051295"/>
+        <c:axId val="321536767"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1246,7 +1817,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="136882127"/>
+        <c:crossAx val="317453567"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1254,7 +1825,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="136882127"/>
+        <c:axId val="317453567"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1305,7 +1876,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="137051295"/>
+        <c:crossAx val="321536767"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3064,23 +3635,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>755650</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>577850</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="9" name="Chart 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{721E96ED-1FDE-324A-9122-D097CCB676D2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62B5511E-61BC-0E4B-B9FA-00C8ACF64F82}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3100,23 +3671,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>787400</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>374650</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
+        <xdr:cNvPr id="15" name="Chart 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D6DF67D-4373-574C-A146-B1C9CFC1BAAA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E8AD2DA-C1B8-0D46-8D85-835BE706D954}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3136,23 +3707,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>838200</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7">
+        <xdr:cNvPr id="16" name="Chart 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E5AEB4F-A54F-D24D-9D87-644EEFEB5C49}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AFBA460-45C7-754F-9C0B-8770967D1FB8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3495,10 +4066,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W6"/>
+  <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3509,49 +4080,49 @@
     <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.6640625" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" customWidth="1"/>
     <col min="22" max="22" width="12.1640625" customWidth="1"/>
     <col min="23" max="23" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="G1" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
       <c r="R1" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S1" s="5"/>
       <c r="T1" s="5"/>
@@ -3581,7 +4152,7 @@
         <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H2" s="1">
         <v>1</v>
@@ -3628,164 +4199,373 @@
       <c r="V2" s="1">
         <v>50</v>
       </c>
-      <c r="W2" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="W2" s="3"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="G3" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="H3" s="1">
-        <v>120770</v>
+        <v>107488</v>
       </c>
       <c r="I3" s="1">
-        <v>121987</v>
+        <v>116416</v>
       </c>
       <c r="J3" s="1">
-        <v>130640</v>
+        <v>123916</v>
       </c>
       <c r="K3" s="1">
-        <v>251209</v>
+        <v>239546</v>
       </c>
       <c r="L3" s="1">
-        <v>582718</v>
+        <v>542936</v>
       </c>
       <c r="M3" s="1">
-        <v>62822</v>
+        <v>24525</v>
       </c>
       <c r="N3" s="1">
-        <v>200872</v>
+        <v>957935</v>
       </c>
       <c r="O3" s="1">
-        <v>388418</v>
+        <v>2568244</v>
       </c>
       <c r="P3" s="1">
-        <v>511396</v>
+        <v>2050420</v>
       </c>
       <c r="Q3" s="1">
-        <v>1387242</v>
+        <v>1949150</v>
       </c>
       <c r="R3" s="1">
-        <v>23438</v>
+        <v>33977807</v>
       </c>
       <c r="S3" s="1">
-        <v>8453</v>
+        <v>8471</v>
       </c>
       <c r="T3" s="1">
-        <v>12235</v>
+        <v>602050</v>
       </c>
       <c r="U3" s="1">
-        <v>19248</v>
+        <v>6456</v>
       </c>
       <c r="V3" s="1">
-        <v>136097</v>
+        <v>15254</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="G4" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="H4" s="1">
-        <f>H3/H2/5000/4</f>
-        <v>6.0385</v>
+        <v>26872</v>
       </c>
       <c r="I4" s="1">
-        <f>I3/I2/5000/4</f>
-        <v>1.21987</v>
+        <v>5820</v>
       </c>
       <c r="J4" s="1">
-        <f>J3/J2/5000/4</f>
-        <v>0.6532</v>
+        <v>3097</v>
       </c>
       <c r="K4" s="1">
-        <f>K3/K2/5000/4</f>
-        <v>0.62802250000000004</v>
+        <v>2994</v>
       </c>
       <c r="L4" s="1">
-        <f>L3/L2/5000/4</f>
-        <v>0.58271800000000007</v>
+        <v>2714</v>
       </c>
       <c r="M4" s="1">
-        <f>M3/M2/10</f>
-        <v>6282.2</v>
+        <v>2452</v>
       </c>
       <c r="N4" s="1">
-        <f>N3/N2/10</f>
-        <v>4017.44</v>
+        <v>22277</v>
       </c>
       <c r="O4" s="1">
-        <f>O3/O2/10</f>
-        <v>3884.1800000000003</v>
+        <v>44280</v>
       </c>
       <c r="P4" s="1">
-        <f>P3/P2/10</f>
-        <v>2556.98</v>
+        <v>25005</v>
       </c>
       <c r="Q4" s="1">
-        <f>Q3/Q2/10</f>
-        <v>2774.4839999999999</v>
+        <v>4836</v>
       </c>
       <c r="R4" s="1">
-        <f>R3/R2/10</f>
-        <v>2343.8000000000002</v>
+        <v>3397780</v>
       </c>
       <c r="S4" s="1">
-        <f>S3/S2/10</f>
-        <v>169.06</v>
+        <v>169</v>
       </c>
       <c r="T4" s="1">
-        <f>T3/T2/10</f>
-        <v>122.35</v>
+        <v>6841</v>
       </c>
       <c r="U4" s="1">
-        <f>U3/U2/10</f>
-        <v>96.24</v>
+        <v>32</v>
       </c>
       <c r="V4" s="1">
-        <f>V3/V2/10</f>
-        <v>272.19400000000002</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>64</v>
-      </c>
-      <c r="B5" s="1">
-        <v>256</v>
-      </c>
-      <c r="C5" s="1">
-        <v>160</v>
-      </c>
-      <c r="D5" s="1">
-        <v>4</v>
-      </c>
-      <c r="E5" s="1">
-        <v>64</v>
-      </c>
-      <c r="F5" s="1">
-        <v>28</v>
+      <c r="G5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="1">
+        <v>104723</v>
+      </c>
+      <c r="I5" s="1">
+        <v>561480</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1190847</v>
+      </c>
+      <c r="K5" s="1">
+        <v>4269171</v>
+      </c>
+      <c r="L5" s="1">
+        <v>18024779</v>
+      </c>
+      <c r="M5" s="1">
+        <v>23604</v>
+      </c>
+      <c r="N5" s="1">
+        <v>505068</v>
+      </c>
+      <c r="O5" s="1">
+        <v>3285498</v>
+      </c>
+      <c r="P5" s="1">
+        <v>5219440</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>18811796</v>
+      </c>
+      <c r="R5" s="1">
+        <v>827</v>
+      </c>
+      <c r="S5" s="1">
+        <v>16475</v>
+      </c>
+      <c r="T5" s="1">
+        <v>18142</v>
+      </c>
+      <c r="U5" s="1">
+        <v>48298</v>
+      </c>
+      <c r="V5" s="1">
+        <v>184009</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+      <c r="G6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
-        <v>36</v>
-      </c>
-      <c r="C6" s="1">
+      <c r="I6" s="1">
         <v>20</v>
       </c>
-      <c r="D6" s="1">
-        <v>4</v>
-      </c>
-      <c r="E6" s="1">
-        <v>8</v>
-      </c>
-      <c r="F6" s="1">
-        <v>4</v>
-      </c>
+      <c r="J6" s="1">
+        <v>40</v>
+      </c>
+      <c r="K6" s="1">
+        <v>80</v>
+      </c>
+      <c r="L6" s="1">
+        <v>200</v>
+      </c>
+      <c r="M6" s="1">
+        <v>10</v>
+      </c>
+      <c r="N6" s="1">
+        <v>43</v>
+      </c>
+      <c r="O6" s="1">
+        <v>58</v>
+      </c>
+      <c r="P6" s="1">
+        <v>82</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>403</v>
+      </c>
+      <c r="R6" s="1">
+        <v>10</v>
+      </c>
+      <c r="S6" s="1">
+        <v>50</v>
+      </c>
+      <c r="T6" s="1">
+        <v>88</v>
+      </c>
+      <c r="U6" s="1">
+        <v>200</v>
+      </c>
+      <c r="V6" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="G7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="1">
+        <v>26180</v>
+      </c>
+      <c r="I7" s="1">
+        <v>28074</v>
+      </c>
+      <c r="J7" s="1">
+        <v>29771</v>
+      </c>
+      <c r="K7" s="1">
+        <v>53364</v>
+      </c>
+      <c r="L7" s="1">
+        <v>90123</v>
+      </c>
+      <c r="M7" s="1">
+        <v>2360</v>
+      </c>
+      <c r="N7" s="1">
+        <v>11745</v>
+      </c>
+      <c r="O7" s="1">
+        <v>56646</v>
+      </c>
+      <c r="P7" s="1">
+        <v>63651</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>46679</v>
+      </c>
+      <c r="R7" s="1">
+        <v>82</v>
+      </c>
+      <c r="S7" s="1">
+        <v>329</v>
+      </c>
+      <c r="T7" s="1">
+        <v>206</v>
+      </c>
+      <c r="U7" s="1">
+        <v>241</v>
+      </c>
+      <c r="V7" s="1">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="G8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="1">
+        <v>28253</v>
+      </c>
+      <c r="I8" s="1">
+        <v>29664</v>
+      </c>
+      <c r="J8" s="1">
+        <v>32226</v>
+      </c>
+      <c r="K8" s="1">
+        <v>86916</v>
+      </c>
+      <c r="L8" s="1">
+        <v>138099</v>
+      </c>
+      <c r="M8" s="1">
+        <v>3809</v>
+      </c>
+      <c r="N8" s="1">
+        <v>351279</v>
+      </c>
+      <c r="O8" s="1">
+        <v>473618</v>
+      </c>
+      <c r="P8" s="1">
+        <v>587264</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>565492</v>
+      </c>
+      <c r="R8" s="1">
+        <v>156</v>
+      </c>
+      <c r="S8" s="1">
+        <v>1796</v>
+      </c>
+      <c r="T8" s="1">
+        <v>1481</v>
+      </c>
+      <c r="U8" s="1">
+        <v>1700</v>
+      </c>
+      <c r="V8" s="1">
+        <v>3843</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="G9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="1">
+        <v>24129</v>
+      </c>
+      <c r="I9" s="1">
+        <v>25778</v>
+      </c>
+      <c r="J9" s="1">
+        <v>27654</v>
+      </c>
+      <c r="K9" s="1">
+        <v>33259</v>
+      </c>
+      <c r="L9" s="1">
+        <v>29712</v>
+      </c>
+      <c r="M9" s="1">
+        <v>1399</v>
+      </c>
+      <c r="N9" s="1">
+        <v>1333</v>
+      </c>
+      <c r="O9" s="1">
+        <v>1464</v>
+      </c>
+      <c r="P9" s="1">
+        <v>3770</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>5432</v>
+      </c>
+      <c r="R9" s="1">
+        <v>49</v>
+      </c>
+      <c r="S9" s="1">
+        <v>38</v>
+      </c>
+      <c r="T9" s="1">
+        <v>37</v>
+      </c>
+      <c r="U9" s="1">
+        <v>35</v>
+      </c>
+      <c r="V9" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
improvements on the reporting format, now reporting call sizes and individual calls
</commit_message>
<xml_diff>
--- a/openbis_benchmark/conf/results.xlsx
+++ b/openbis_benchmark/conf/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanf/Documents/programming/openbis_eclipse_workspace_git/openbis_benchmark/conf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F25E2D50-2A7E-A646-AC71-9FF0D3A74A0C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BFB14549-F674-0F4E-865A-F5B7C425B067}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29360" yWindow="460" windowWidth="50100" windowHeight="26140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="460" windowWidth="30560" windowHeight="21060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>16
 shared_buffers 4GB
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>SEARCH</t>
-  </si>
-  <si>
-    <t>QUERY</t>
   </si>
   <si>
     <t>RESULTS</t>
@@ -97,12 +94,18 @@
   <si>
     <t>MIN OPERATION TIME</t>
   </si>
+  <si>
+    <t>QUERY - Original</t>
+  </si>
+  <si>
+    <t>QUERY - Corrected</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -130,14 +133,6 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -177,7 +172,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -185,7 +180,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -994,8 +988,89 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TOTAL REAL TIME</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$R$2:$V$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$3:$V$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8471</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6456</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15254</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-48C7-0942-80F1-69F959A7CD91}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$G$7</c:f>
@@ -1076,7 +1151,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$G$8</c:f>
@@ -1157,7 +1232,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$G$9</c:f>
@@ -1519,8 +1594,89 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TOTAL REAL TIME</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$M$2:$Q$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$3:$Q$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>24525</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>957935</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2568244</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2050420</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1949150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B2B1-5448-9B7B-27D2E39801B8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$G$7</c:f>
@@ -1601,7 +1757,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$G$8</c:f>
@@ -1682,7 +1838,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$G$9</c:f>
@@ -3671,14 +3827,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>374650</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>806450</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -3713,8 +3869,8 @@
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
@@ -4066,10 +4222,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W12"/>
+  <dimension ref="A1:AB12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+    <sheetView tabSelected="1" topLeftCell="Q6" zoomScale="155" zoomScaleNormal="155" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4085,54 +4241,61 @@
     <col min="23" max="23" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="5" t="s">
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5" t="s">
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
       <c r="W1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="192" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" ht="192" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>16</v>
       </c>
@@ -4152,7 +4315,7 @@
         <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H2" s="1">
         <v>1</v>
@@ -4199,11 +4362,25 @@
       <c r="V2" s="1">
         <v>50</v>
       </c>
-      <c r="W2" s="3"/>
+      <c r="W2" s="1">
+        <v>1</v>
+      </c>
+      <c r="X2" s="1">
+        <v>5</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>10</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>20</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>50</v>
+      </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="G3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3" s="1">
         <v>107488</v>
@@ -4236,13 +4413,13 @@
         <v>1949150</v>
       </c>
       <c r="R3" s="1">
-        <v>33977807</v>
+        <v>0</v>
       </c>
       <c r="S3" s="1">
         <v>8471</v>
       </c>
       <c r="T3" s="1">
-        <v>602050</v>
+        <v>0</v>
       </c>
       <c r="U3" s="1">
         <v>6456</v>
@@ -4250,10 +4427,25 @@
       <c r="V3" s="1">
         <v>15254</v>
       </c>
+      <c r="W3" s="1">
+        <v>33977807</v>
+      </c>
+      <c r="X3" s="1">
+        <v>8471</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>602050</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>6456</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>15254</v>
+      </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="G4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H4" s="1">
         <v>26872</v>
@@ -4300,10 +4492,25 @@
       <c r="V4" s="1">
         <v>30</v>
       </c>
+      <c r="W4" s="1">
+        <v>3397780</v>
+      </c>
+      <c r="X4" s="1">
+        <v>169</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>6841</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>32</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>30</v>
+      </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="G5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H5" s="1">
         <v>104723</v>
@@ -4350,10 +4557,25 @@
       <c r="V5" s="1">
         <v>184009</v>
       </c>
+      <c r="W5" s="1">
+        <v>827</v>
+      </c>
+      <c r="X5" s="1">
+        <v>16475</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>18142</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>48298</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>184009</v>
+      </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="G6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H6" s="1">
         <v>4</v>
@@ -4400,10 +4622,25 @@
       <c r="V6" s="1">
         <v>500</v>
       </c>
+      <c r="W6" s="1">
+        <v>10</v>
+      </c>
+      <c r="X6" s="1">
+        <v>50</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>88</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>200</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>500</v>
+      </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="G7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H7" s="1">
         <v>26180</v>
@@ -4450,10 +4687,25 @@
       <c r="V7" s="1">
         <v>368</v>
       </c>
+      <c r="W7" s="1">
+        <v>82</v>
+      </c>
+      <c r="X7" s="1">
+        <v>329</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>206</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>241</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>368</v>
+      </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="G8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H8" s="1">
         <v>28253</v>
@@ -4500,10 +4752,25 @@
       <c r="V8" s="1">
         <v>3843</v>
       </c>
+      <c r="W8" s="1">
+        <v>156</v>
+      </c>
+      <c r="X8" s="1">
+        <v>1796</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>1481</v>
+      </c>
+      <c r="Z8" s="1">
+        <v>1700</v>
+      </c>
+      <c r="AA8" s="1">
+        <v>3843</v>
+      </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="G9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H9" s="1">
         <v>24129</v>
@@ -4550,8 +4817,23 @@
       <c r="V9" s="1">
         <v>24</v>
       </c>
+      <c r="W9" s="1">
+        <v>49</v>
+      </c>
+      <c r="X9" s="1">
+        <v>38</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>37</v>
+      </c>
+      <c r="Z9" s="1">
+        <v>35</v>
+      </c>
+      <c r="AA9" s="1">
+        <v>24</v>
+      </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -4559,7 +4841,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -4568,10 +4850,11 @@
       <c r="F12" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="H1:L1"/>
     <mergeCell ref="M1:Q1"/>
     <mergeCell ref="R1:V1"/>
+    <mergeCell ref="W1:AA1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>